<commit_message>
add cheques collections interface
</commit_message>
<xml_diff>
--- a/elsawy_cheques_testcases.xlsx
+++ b/elsawy_cheques_testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed.El-Sawy\Documents\cheque collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F063EEB-2A6E-4231-BCDC-04FC8FDA57DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085D83BE-2344-4A4C-A533-0D5E2AFA4E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9097CBEB-AA54-4FBA-956C-ABD4568C22BC}"/>
   </bookViews>
@@ -2707,11 +2707,6 @@
 3. Format of data confirmed </t>
   </si>
   <si>
-    <t xml:space="preserve"> 1. Filter applied 
-2. Matching record(s) shown 
-3. Amounts and balances correct </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1. Account info shown 
 2. Balance after debit is negative 
 3. System computed value matches </t>
@@ -2726,11 +2721,6 @@
     <t xml:space="preserve"> Account No: 0360000983843. </t>
   </si>
   <si>
-    <t xml:space="preserve"> 1. Files shown by date 
-2. Details include user, size, time 
-3. All files downloadable </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1. Click on رفض (Reject) 
 2. Input reason in textbox 
 3. Click Submit </t>
@@ -2762,11 +2752,6 @@
     <t xml:space="preserve"> 1. File goes from Pending to Sent 
 2. Service logs updated 
 3. File archived </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1. Entry deleted 
-2. Log message saved 
-3. File/files cleared from storage </t>
   </si>
   <si>
     <t xml:space="preserve"> Ref: 11403603. </t>
@@ -2952,12 +2937,6 @@
 4. Review status, timestamps </t>
   </si>
   <si>
-    <t xml:space="preserve"> 1. File found 
-2. Status displayed (e.g., AUTH) 
-3. Timestamp + metadata correct 
-4. Batch traceable </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1. Login to E.NOF.CHQ.2. 
 2. Input file name 
 3. Search 
@@ -3213,18 +3192,6 @@
 4. Entry locked post-confirm </t>
   </si>
   <si>
-    <t xml:space="preserve"> 1. Request marked as Rejected 
-2. Reason saved 
-3. Color/status updated in UI 
-4. Locked for editing </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1. File uploaded 
-2. Icon shown in request row 
-3. Size + date shown 
-4. File downloadable </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1. Open audit log screen 
 2. Enter request ref no 
 3. Click Search 
@@ -3277,12 +3244,6 @@
 2. Amount = 2,000,000.00 
 3. PDF advice &amp; fields accurate 
 4. Ref and status = complete </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1. Files open in viewer 
-2. Unit size shown correctly 
-3. Name = expected 
-4. Download if needed </t>
   </si>
   <si>
     <t xml:space="preserve"> INI_CCHQ_74. </t>
@@ -4375,6 +4336,50 @@
   </si>
   <si>
     <t xml:space="preserve"> Date=20250707. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. loged in 
+ 2. Filter applied 
+3. Matching record(s) shown 
+4. Amounts and balances correct </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. loged in 
+ 2. File found 
+3. Status displayed (e.g., AUTH) 
+4. Timestamp + metadata correct 
+4. Batch traceable </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. loged in 
+2. Files shown by date 
+3. Details include user, size, time 
+4. All files downloadable </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Request marked as Rejected 
+2. Reason saved 
+3. Color/status updated in UI 
+and Locked for editing </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. File uploaded 
+2. Icon shown in request row 
+3. Size + date shown 
+and File downloadable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, Located unapproved SWIFT row  
+2. Entry deleted 
+3. Log message saved 
+4. File/files cleared from storage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. navigated 
+2. Files open in viewer 
+3. Unit size shown correctly 
+4. Name = expected 
+5. Download if needed </t>
   </si>
 </sst>
 </file>
@@ -4805,8 +4810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F05374B-CEAB-4E57-A6E8-AE01898F8810}">
   <dimension ref="A1:R128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H3" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="M124" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O130" sqref="O130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="66.33203125" defaultRowHeight="14.4"/>
@@ -4921,16 +4926,16 @@
         <v>6</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>1123</v>
+        <v>1116</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>1137</v>
+        <v>1130</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>1124</v>
+        <v>1117</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>20</v>
@@ -4973,16 +4978,16 @@
         <v>6</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>1125</v>
+        <v>1118</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>1138</v>
+        <v>1131</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>1126</v>
+        <v>1119</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>24</v>
@@ -5025,16 +5030,16 @@
         <v>6</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>1003</v>
+        <v>996</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>1139</v>
+        <v>1132</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>1004</v>
+        <v>997</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>28</v>
@@ -5077,16 +5082,16 @@
         <v>6</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>1005</v>
+        <v>998</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>1140</v>
+        <v>1133</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>1006</v>
+        <v>999</v>
       </c>
       <c r="P5" s="4" t="s">
         <v>32</v>
@@ -5129,16 +5134,16 @@
         <v>6</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>1007</v>
+        <v>1000</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>1008</v>
+        <v>1001</v>
       </c>
       <c r="P6" s="4" t="s">
         <v>36</v>
@@ -5181,16 +5186,16 @@
         <v>6</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>1009</v>
+        <v>1002</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>1141</v>
+        <v>1134</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>1010</v>
+        <v>1003</v>
       </c>
       <c r="P7" s="4" t="s">
         <v>40</v>
@@ -5233,16 +5238,16 @@
         <v>6</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>1011</v>
+        <v>1004</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>1139</v>
+        <v>1132</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>1012</v>
+        <v>1005</v>
       </c>
       <c r="P8" s="4" t="s">
         <v>44</v>
@@ -5285,16 +5290,16 @@
         <v>6</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="P9" s="4" t="s">
         <v>48</v>
@@ -5337,16 +5342,16 @@
         <v>6</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="N10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="P10" s="4" t="s">
         <v>52</v>
@@ -5374,7 +5379,7 @@
         <v>54</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>1013</v>
+        <v>1006</v>
       </c>
       <c r="H11" s="4">
         <v>1000</v>
@@ -5389,16 +5394,16 @@
         <v>6</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>1014</v>
+        <v>1007</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>1015</v>
+        <v>1008</v>
       </c>
       <c r="P11" s="4" t="s">
         <v>56</v>
@@ -5441,16 +5446,16 @@
         <v>6</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>1016</v>
+        <v>1009</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>1139</v>
+        <v>1132</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>1017</v>
+        <v>1010</v>
       </c>
       <c r="P12" s="4" t="s">
         <v>60</v>
@@ -5493,16 +5498,16 @@
         <v>6</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>833</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="P13" s="4" t="s">
         <v>64</v>
@@ -5545,16 +5550,16 @@
         <v>6</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>1142</v>
+        <v>1135</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="P14" s="4" t="s">
         <v>68</v>
@@ -5597,16 +5602,16 @@
         <v>6</v>
       </c>
       <c r="L15" s="4" t="s">
+        <v>1129</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>1011</v>
+      </c>
+      <c r="N15" s="4" t="s">
         <v>1136</v>
       </c>
-      <c r="M15" s="4" t="s">
-        <v>1018</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>1143</v>
-      </c>
       <c r="O15" s="4" t="s">
-        <v>1019</v>
+        <v>1012</v>
       </c>
       <c r="P15" s="4" t="s">
         <v>72</v>
@@ -5649,7 +5654,7 @@
         <v>6</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>852</v>
@@ -5701,13 +5706,13 @@
         <v>6</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>854</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>1143</v>
+        <v>1136</v>
       </c>
       <c r="O17" s="4" t="s">
         <v>855</v>
@@ -5738,7 +5743,7 @@
         <v>81</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>1127</v>
+        <v>1120</v>
       </c>
       <c r="H18" s="4">
         <v>1000</v>
@@ -5753,7 +5758,7 @@
         <v>6</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>856</v>
@@ -5790,7 +5795,7 @@
         <v>85</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>1144</v>
+        <v>1137</v>
       </c>
       <c r="H19" s="4">
         <v>1000</v>
@@ -5805,7 +5810,7 @@
         <v>6</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>858</v>
@@ -5857,16 +5862,16 @@
         <v>6</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>1145</v>
+        <v>1138</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="P20" s="4" t="s">
         <v>91</v>
@@ -5909,16 +5914,16 @@
         <v>6</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>1146</v>
+        <v>1139</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="P21" s="4" t="s">
         <v>94</v>
@@ -5961,16 +5966,16 @@
         <v>6</v>
       </c>
       <c r="L22" s="4" t="s">
+        <v>1129</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>1013</v>
+      </c>
+      <c r="N22" s="4" t="s">
         <v>1136</v>
       </c>
-      <c r="M22" s="4" t="s">
-        <v>1020</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>1143</v>
-      </c>
       <c r="O22" s="4" t="s">
-        <v>1021</v>
+        <v>1014</v>
       </c>
       <c r="P22" s="4" t="s">
         <v>97</v>
@@ -6013,13 +6018,13 @@
         <v>6</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>860</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>1147</v>
+        <v>1140</v>
       </c>
       <c r="O23" s="4" t="s">
         <v>861</v>
@@ -6065,16 +6070,16 @@
         <v>6</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>104</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="P24" s="4" t="s">
         <v>105</v>
@@ -6117,16 +6122,16 @@
         <v>6</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>1148</v>
+        <v>1141</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="P25" s="4" t="s">
         <v>109</v>
@@ -6154,7 +6159,7 @@
         <v>111</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="H26" s="4">
         <v>1000</v>
@@ -6169,7 +6174,7 @@
         <v>6</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M26" s="4" t="s">
         <v>863</v>
@@ -6206,7 +6211,7 @@
         <v>114</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="H27" s="4">
         <v>1000</v>
@@ -6221,16 +6226,16 @@
         <v>6</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>1128</v>
+        <v>1121</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>116</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>1129</v>
+        <v>1122</v>
       </c>
       <c r="P27" s="4" t="s">
         <v>117</v>
@@ -6258,7 +6263,7 @@
         <v>119</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>1130</v>
+        <v>1123</v>
       </c>
       <c r="H28" s="4">
         <v>1000</v>
@@ -6273,13 +6278,13 @@
         <v>6</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M28" s="4" t="s">
         <v>866</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>1149</v>
+        <v>1142</v>
       </c>
       <c r="O28" s="4" t="s">
         <v>867</v>
@@ -6325,7 +6330,7 @@
         <v>6</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M29" s="4" t="s">
         <v>868</v>
@@ -6377,7 +6382,7 @@
         <v>6</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M30" s="4" t="s">
         <v>870</v>
@@ -6414,7 +6419,7 @@
         <v>132</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>1150</v>
+        <v>1143</v>
       </c>
       <c r="H31" s="4">
         <v>1000</v>
@@ -6429,16 +6434,16 @@
         <v>6</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>1151</v>
+        <v>1144</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="P31" s="4" t="s">
         <v>134</v>
@@ -6481,16 +6486,16 @@
         <v>6</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>17</v>
       </c>
       <c r="O32" s="4" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="P32" s="4" t="s">
         <v>138</v>
@@ -6533,16 +6538,16 @@
         <v>6</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>142</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="P33" s="4" t="s">
         <v>143</v>
@@ -6585,16 +6590,16 @@
         <v>6</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>147</v>
       </c>
       <c r="O34" s="4" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="P34" s="4" t="s">
         <v>148</v>
@@ -6637,7 +6642,7 @@
         <v>6</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M35" s="4" t="s">
         <v>873</v>
@@ -6689,16 +6694,16 @@
         <v>6</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>152</v>
       </c>
       <c r="O36" s="4" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="P36" s="4" t="s">
         <v>153</v>
@@ -6726,7 +6731,7 @@
         <v>155</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>1150</v>
+        <v>1143</v>
       </c>
       <c r="H37" s="4">
         <v>1000</v>
@@ -6741,16 +6746,16 @@
         <v>6</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>1022</v>
+        <v>1015</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>157</v>
       </c>
       <c r="O37" s="4" t="s">
-        <v>1023</v>
+        <v>1016</v>
       </c>
       <c r="P37" s="4" t="s">
         <v>158</v>
@@ -6778,7 +6783,7 @@
         <v>160</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>1131</v>
+        <v>1124</v>
       </c>
       <c r="H38" s="4">
         <v>1000</v>
@@ -6793,16 +6798,16 @@
         <v>6</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="N38" s="4" t="s">
         <v>161</v>
       </c>
       <c r="O38" s="4" t="s">
-        <v>875</v>
+        <v>1153</v>
       </c>
       <c r="P38" s="4" t="s">
         <v>162</v>
@@ -6830,7 +6835,7 @@
         <v>164</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>1131</v>
+        <v>1124</v>
       </c>
       <c r="H39" s="4">
         <v>1000</v>
@@ -6845,16 +6850,16 @@
         <v>6</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>1139</v>
+        <v>1132</v>
       </c>
       <c r="O39" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="P39" s="4" t="s">
         <v>165</v>
@@ -6862,7 +6867,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="40" spans="1:18" ht="55.2">
+    <row r="40" spans="1:18" ht="69">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -6897,16 +6902,16 @@
         <v>6</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="N40" s="4" t="s">
         <v>169</v>
       </c>
       <c r="O40" s="4" t="s">
-        <v>921</v>
+        <v>1154</v>
       </c>
       <c r="P40" s="4" t="s">
         <v>170</v>
@@ -6949,16 +6954,16 @@
         <v>6</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>171</v>
       </c>
       <c r="O41" s="4" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
       <c r="P41" s="4" t="s">
         <v>845</v>
@@ -6986,7 +6991,7 @@
         <v>174</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>1024</v>
+        <v>1017</v>
       </c>
       <c r="H42" s="4">
         <v>1000</v>
@@ -7001,16 +7006,16 @@
         <v>6</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>924</v>
+        <v>920</v>
       </c>
       <c r="N42" s="4" t="s">
         <v>176</v>
       </c>
       <c r="O42" s="4" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="P42" s="4" t="s">
         <v>177</v>
@@ -7029,7 +7034,7 @@
         <v>747</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>926</v>
+        <v>922</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>2</v>
@@ -7053,19 +7058,19 @@
         <v>6</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
       <c r="N43" s="4" t="s">
-        <v>1025</v>
+        <v>1018</v>
       </c>
       <c r="O43" s="4" t="s">
-        <v>928</v>
+        <v>924</v>
       </c>
       <c r="P43" s="4" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
@@ -7105,16 +7110,16 @@
         <v>6</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="O44" s="4" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
       <c r="P44" s="4" t="s">
         <v>182</v>
@@ -7157,16 +7162,16 @@
         <v>6</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>185</v>
       </c>
       <c r="O45" s="4" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
       <c r="P45" s="4" t="s">
         <v>186</v>
@@ -7194,7 +7199,7 @@
         <v>188</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
       <c r="H46" s="4">
         <v>1000</v>
@@ -7203,22 +7208,22 @@
         <v>5</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="K46" s="4" t="s">
         <v>6</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
       <c r="O46" s="4" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="P46" s="4" t="s">
         <v>189</v>
@@ -7264,13 +7269,13 @@
         <v>193</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>194</v>
       </c>
       <c r="O47" s="4" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="P47" s="4" t="s">
         <v>195</v>
@@ -7316,13 +7321,13 @@
         <v>193</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>199</v>
       </c>
       <c r="O48" s="4" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
       <c r="P48" s="4" t="s">
         <v>200</v>
@@ -7368,13 +7373,13 @@
         <v>193</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
       <c r="N49" s="4" t="s">
-        <v>1026</v>
+        <v>1019</v>
       </c>
       <c r="O49" s="4" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
       <c r="P49" s="4" t="s">
         <v>204</v>
@@ -7420,13 +7425,13 @@
         <v>193</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>207</v>
       </c>
       <c r="O50" s="4" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
       <c r="P50" s="4" t="s">
         <v>208</v>
@@ -7454,7 +7459,7 @@
         <v>211</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
       <c r="H51" s="4">
         <v>1000</v>
@@ -7472,13 +7477,13 @@
         <v>193</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>946</v>
+        <v>942</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>213</v>
       </c>
       <c r="O51" s="4" t="s">
-        <v>947</v>
+        <v>943</v>
       </c>
       <c r="P51" s="4" t="s">
         <v>214</v>
@@ -7524,13 +7529,13 @@
         <v>193</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>1152</v>
+        <v>1145</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>949</v>
+        <v>945</v>
       </c>
       <c r="P52" s="2" t="s">
         <v>219</v>
@@ -7574,13 +7579,13 @@
         <v>193</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
       <c r="N53" s="2" t="s">
         <v>17</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>951</v>
+        <v>947</v>
       </c>
       <c r="P53" s="2" t="s">
         <v>223</v>
@@ -7624,13 +7629,13 @@
         <v>193</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>952</v>
+        <v>948</v>
       </c>
       <c r="N54" s="2" t="s">
         <v>227</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>953</v>
+        <v>949</v>
       </c>
       <c r="P54" s="2" t="s">
         <v>228</v>
@@ -7674,13 +7679,13 @@
         <v>193</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
       <c r="P55" s="2" t="s">
         <v>232</v>
@@ -7706,7 +7711,7 @@
         <v>252</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>1132</v>
+        <v>1125</v>
       </c>
       <c r="H56" s="2">
         <v>1000</v>
@@ -7724,13 +7729,13 @@
         <v>250</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>1027</v>
+        <v>1020</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>1153</v>
+        <v>1146</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="P56" s="2" t="s">
         <v>254</v>
@@ -7756,7 +7761,7 @@
         <v>256</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>1013</v>
+        <v>1006</v>
       </c>
       <c r="H57" s="2">
         <v>1000</v>
@@ -7774,13 +7779,13 @@
         <v>250</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>1028</v>
+        <v>1021</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
       <c r="O57" s="2" t="s">
-        <v>958</v>
+        <v>954</v>
       </c>
       <c r="P57" s="2" t="s">
         <v>258</v>
@@ -7824,13 +7829,13 @@
         <v>250</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>959</v>
+        <v>955</v>
       </c>
       <c r="N58" s="2" t="s">
         <v>263</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
       <c r="P58" s="2" t="s">
         <v>264</v>
@@ -7874,13 +7879,13 @@
         <v>250</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>1154</v>
+        <v>1147</v>
       </c>
       <c r="O59" s="2" t="s">
-        <v>880</v>
+        <v>1155</v>
       </c>
       <c r="P59" s="2" t="s">
         <v>268</v>
@@ -7924,7 +7929,7 @@
         <v>250</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="N60" s="2" t="s">
         <v>273</v>
@@ -7974,13 +7979,13 @@
         <v>250</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="N61" s="2" t="s">
         <v>277</v>
       </c>
       <c r="O61" s="2" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="P61" s="2" t="s">
         <v>278</v>
@@ -8024,13 +8029,13 @@
         <v>250</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>965</v>
+        <v>961</v>
       </c>
       <c r="N62" s="2" t="s">
         <v>281</v>
       </c>
       <c r="O62" s="2" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
       <c r="P62" s="2" t="s">
         <v>282</v>
@@ -8074,13 +8079,13 @@
         <v>250</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="N63" s="2" t="s">
         <v>285</v>
       </c>
       <c r="O63" s="2" t="s">
-        <v>967</v>
+        <v>1156</v>
       </c>
       <c r="P63" s="2" t="s">
         <v>286</v>
@@ -8124,13 +8129,13 @@
         <v>250</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>1029</v>
+        <v>1022</v>
       </c>
       <c r="O64" s="2" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="P64" s="2" t="s">
         <v>289</v>
@@ -8174,13 +8179,13 @@
         <v>250</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="N65" s="2" t="s">
         <v>292</v>
       </c>
       <c r="O65" s="2" t="s">
-        <v>968</v>
+        <v>1157</v>
       </c>
       <c r="P65" s="2" t="s">
         <v>293</v>
@@ -8206,7 +8211,7 @@
         <v>295</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="H66" s="2">
         <v>1000</v>
@@ -8224,13 +8229,13 @@
         <v>250</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>969</v>
+        <v>963</v>
       </c>
       <c r="N66" s="2" t="s">
         <v>297</v>
       </c>
       <c r="O66" s="2" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
       <c r="P66" s="2" t="s">
         <v>298</v>
@@ -8256,7 +8261,7 @@
         <v>301</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="H67" s="2">
         <v>1000</v>
@@ -8274,13 +8279,13 @@
         <v>250</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="N67" s="2" t="s">
         <v>303</v>
       </c>
       <c r="O67" s="2" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="P67" s="2" t="s">
         <v>304</v>
@@ -8324,13 +8329,13 @@
         <v>250</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="N68" s="2" t="s">
         <v>308</v>
       </c>
       <c r="O68" s="2" t="s">
-        <v>888</v>
+        <v>1158</v>
       </c>
       <c r="P68" s="2" t="s">
         <v>309</v>
@@ -8374,13 +8379,13 @@
         <v>250</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
       <c r="N69" s="2" t="s">
         <v>314</v>
       </c>
       <c r="O69" s="2" t="s">
-        <v>973</v>
+        <v>967</v>
       </c>
       <c r="P69" s="2" t="s">
         <v>315</v>
@@ -8424,13 +8429,13 @@
         <v>317</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>974</v>
+        <v>968</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>975</v>
+        <v>969</v>
       </c>
       <c r="P70" s="2" t="s">
         <v>320</v>
@@ -8456,7 +8461,7 @@
         <v>322</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="H71" s="2">
         <v>1000</v>
@@ -8474,13 +8479,13 @@
         <v>317</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>976</v>
+        <v>970</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>1133</v>
+        <v>1126</v>
       </c>
       <c r="O71" s="2" t="s">
-        <v>977</v>
+        <v>971</v>
       </c>
       <c r="P71" s="2" t="s">
         <v>323</v>
@@ -8506,7 +8511,7 @@
         <v>325</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="H72" s="2">
         <v>1000</v>
@@ -8524,13 +8529,13 @@
         <v>317</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>1030</v>
+        <v>1023</v>
       </c>
       <c r="N72" s="2" t="s">
         <v>326</v>
       </c>
       <c r="O72" s="2" t="s">
-        <v>978</v>
+        <v>1159</v>
       </c>
       <c r="P72" s="2" t="s">
         <v>327</v>
@@ -8556,7 +8561,7 @@
         <v>329</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>979</v>
+        <v>972</v>
       </c>
       <c r="H73" s="2">
         <v>1000</v>
@@ -8574,13 +8579,13 @@
         <v>317</v>
       </c>
       <c r="M73" s="2" t="s">
-        <v>980</v>
+        <v>973</v>
       </c>
       <c r="N73" s="2" t="s">
         <v>330</v>
       </c>
       <c r="O73" s="2" t="s">
-        <v>981</v>
+        <v>974</v>
       </c>
       <c r="P73" s="2" t="s">
         <v>331</v>
@@ -8624,13 +8629,13 @@
         <v>317</v>
       </c>
       <c r="M74" s="2" t="s">
-        <v>982</v>
+        <v>975</v>
       </c>
       <c r="N74" s="2" t="s">
         <v>334</v>
       </c>
       <c r="O74" s="2" t="s">
-        <v>983</v>
+        <v>976</v>
       </c>
       <c r="P74" s="2" t="s">
         <v>335</v>
@@ -8656,7 +8661,7 @@
         <v>337</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>1031</v>
+        <v>1024</v>
       </c>
       <c r="H75" s="2">
         <v>1000</v>
@@ -8674,13 +8679,13 @@
         <v>317</v>
       </c>
       <c r="M75" s="2" t="s">
-        <v>984</v>
+        <v>977</v>
       </c>
       <c r="N75" s="2" t="s">
         <v>338</v>
       </c>
       <c r="O75" s="2" t="s">
-        <v>985</v>
+        <v>978</v>
       </c>
       <c r="P75" s="2" t="s">
         <v>339</v>
@@ -8706,7 +8711,7 @@
         <v>341</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>1134</v>
+        <v>1127</v>
       </c>
       <c r="H76" s="2">
         <v>1000</v>
@@ -8724,13 +8729,13 @@
         <v>317</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>986</v>
+        <v>979</v>
       </c>
       <c r="N76" s="2" t="s">
         <v>835</v>
       </c>
       <c r="O76" s="2" t="s">
-        <v>987</v>
+        <v>980</v>
       </c>
       <c r="P76" s="2" t="s">
         <v>342</v>
@@ -8774,13 +8779,13 @@
         <v>317</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>988</v>
+        <v>981</v>
       </c>
       <c r="N77" s="2" t="s">
         <v>345</v>
       </c>
       <c r="O77" s="2" t="s">
-        <v>989</v>
+        <v>982</v>
       </c>
       <c r="P77" s="2" t="s">
         <v>346</v>
@@ -8824,13 +8829,13 @@
         <v>317</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>990</v>
+        <v>983</v>
       </c>
       <c r="N78" s="2" t="s">
         <v>348</v>
       </c>
       <c r="O78" s="2" t="s">
-        <v>991</v>
+        <v>984</v>
       </c>
       <c r="P78" s="2" t="s">
         <v>349</v>
@@ -8874,13 +8879,13 @@
         <v>317</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>992</v>
+        <v>985</v>
       </c>
       <c r="N79" s="2" t="s">
         <v>352</v>
       </c>
       <c r="O79" s="2" t="s">
-        <v>993</v>
+        <v>986</v>
       </c>
       <c r="P79" s="2" t="s">
         <v>353</v>
@@ -8924,13 +8929,13 @@
         <v>317</v>
       </c>
       <c r="M80" s="2" t="s">
-        <v>994</v>
+        <v>987</v>
       </c>
       <c r="N80" s="2" t="s">
         <v>356</v>
       </c>
       <c r="O80" s="2" t="s">
-        <v>995</v>
+        <v>988</v>
       </c>
       <c r="P80" s="2" t="s">
         <v>357</v>
@@ -8974,13 +8979,13 @@
         <v>317</v>
       </c>
       <c r="M81" s="2" t="s">
-        <v>996</v>
+        <v>989</v>
       </c>
       <c r="N81" s="2" t="s">
         <v>360</v>
       </c>
       <c r="O81" s="2" t="s">
-        <v>997</v>
+        <v>990</v>
       </c>
       <c r="P81" s="2" t="s">
         <v>361</v>
@@ -9006,7 +9011,7 @@
         <v>363</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>1155</v>
+        <v>1148</v>
       </c>
       <c r="H82" s="2">
         <v>1000</v>
@@ -9024,13 +9029,13 @@
         <v>317</v>
       </c>
       <c r="M82" s="2" t="s">
-        <v>998</v>
+        <v>991</v>
       </c>
       <c r="N82" s="2" t="s">
         <v>364</v>
       </c>
       <c r="O82" s="2" t="s">
-        <v>999</v>
+        <v>992</v>
       </c>
       <c r="P82" s="2" t="s">
         <v>365</v>
@@ -9056,7 +9061,7 @@
         <v>367</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>1000</v>
+        <v>993</v>
       </c>
       <c r="H83" s="2">
         <v>1000</v>
@@ -9074,13 +9079,13 @@
         <v>317</v>
       </c>
       <c r="M83" s="2" t="s">
-        <v>1001</v>
+        <v>994</v>
       </c>
       <c r="N83" s="2" t="s">
         <v>369</v>
       </c>
       <c r="O83" s="2" t="s">
-        <v>1002</v>
+        <v>995</v>
       </c>
       <c r="P83" s="2" t="s">
         <v>370</v>
@@ -9121,16 +9126,16 @@
         <v>6</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M84" s="2" t="s">
-        <v>1032</v>
+        <v>1025</v>
       </c>
       <c r="N84" s="2" t="s">
         <v>374</v>
       </c>
       <c r="O84" s="2" t="s">
-        <v>1033</v>
+        <v>1026</v>
       </c>
       <c r="P84" s="2" t="s">
         <v>375</v>
@@ -9171,16 +9176,16 @@
         <v>6</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M85" s="2" t="s">
-        <v>1034</v>
+        <v>1027</v>
       </c>
       <c r="N85" s="2" t="s">
         <v>379</v>
       </c>
       <c r="O85" s="2" t="s">
-        <v>1035</v>
+        <v>1028</v>
       </c>
       <c r="P85" s="2" t="s">
         <v>380</v>
@@ -9221,16 +9226,16 @@
         <v>6</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M86" s="2" t="s">
-        <v>1036</v>
+        <v>1029</v>
       </c>
       <c r="N86" s="2" t="s">
         <v>379</v>
       </c>
       <c r="O86" s="2" t="s">
-        <v>1037</v>
+        <v>1030</v>
       </c>
       <c r="P86" s="2" t="s">
         <v>382</v>
@@ -9271,16 +9276,16 @@
         <v>6</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M87" s="2" t="s">
-        <v>1038</v>
+        <v>1031</v>
       </c>
       <c r="N87" s="2" t="s">
         <v>385</v>
       </c>
       <c r="O87" s="2" t="s">
-        <v>1039</v>
+        <v>1032</v>
       </c>
       <c r="P87" s="2" t="s">
         <v>386</v>
@@ -9321,16 +9326,16 @@
         <v>6</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M88" s="2" t="s">
-        <v>1040</v>
+        <v>1033</v>
       </c>
       <c r="N88" s="2" t="s">
         <v>388</v>
       </c>
       <c r="O88" s="2" t="s">
-        <v>1041</v>
+        <v>1034</v>
       </c>
       <c r="P88" s="2" t="s">
         <v>389</v>
@@ -9371,16 +9376,16 @@
         <v>6</v>
       </c>
       <c r="L89" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M89" s="2" t="s">
-        <v>1042</v>
+        <v>1035</v>
       </c>
       <c r="N89" s="2" t="s">
         <v>392</v>
       </c>
       <c r="O89" s="2" t="s">
-        <v>1043</v>
+        <v>1036</v>
       </c>
       <c r="P89" s="2" t="s">
         <v>393</v>
@@ -9421,16 +9426,16 @@
         <v>6</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M90" s="2" t="s">
-        <v>1044</v>
+        <v>1037</v>
       </c>
       <c r="N90" s="2" t="s">
         <v>395</v>
       </c>
       <c r="O90" s="2" t="s">
-        <v>1045</v>
+        <v>1038</v>
       </c>
       <c r="P90" s="2" t="s">
         <v>396</v>
@@ -9471,16 +9476,16 @@
         <v>6</v>
       </c>
       <c r="L91" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M91" s="2" t="s">
-        <v>1046</v>
+        <v>1039</v>
       </c>
       <c r="N91" s="2" t="s">
         <v>398</v>
       </c>
       <c r="O91" s="2" t="s">
-        <v>1047</v>
+        <v>1040</v>
       </c>
       <c r="P91" s="2" t="s">
         <v>399</v>
@@ -9521,16 +9526,16 @@
         <v>6</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M92" s="2" t="s">
-        <v>1048</v>
+        <v>1041</v>
       </c>
       <c r="N92" s="2" t="s">
-        <v>1049</v>
+        <v>1042</v>
       </c>
       <c r="O92" s="2" t="s">
-        <v>1050</v>
+        <v>1043</v>
       </c>
       <c r="P92" s="2" t="s">
         <v>401</v>
@@ -9571,16 +9576,16 @@
         <v>6</v>
       </c>
       <c r="L93" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M93" s="2" t="s">
-        <v>1051</v>
+        <v>1044</v>
       </c>
       <c r="N93" s="2" t="s">
-        <v>1135</v>
+        <v>1128</v>
       </c>
       <c r="O93" s="2" t="s">
-        <v>1052</v>
+        <v>1045</v>
       </c>
       <c r="P93" s="2" t="s">
         <v>403</v>
@@ -9621,16 +9626,16 @@
         <v>6</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M94" s="2" t="s">
-        <v>1053</v>
+        <v>1046</v>
       </c>
       <c r="N94" s="2" t="s">
         <v>405</v>
       </c>
       <c r="O94" s="2" t="s">
-        <v>1054</v>
+        <v>1047</v>
       </c>
       <c r="P94" s="2" t="s">
         <v>406</v>
@@ -9671,16 +9676,16 @@
         <v>6</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M95" s="2" t="s">
-        <v>1055</v>
+        <v>1048</v>
       </c>
       <c r="N95" s="2" t="s">
         <v>408</v>
       </c>
       <c r="O95" s="2" t="s">
-        <v>1056</v>
+        <v>1049</v>
       </c>
       <c r="P95" s="2" t="s">
         <v>409</v>
@@ -9721,16 +9726,16 @@
         <v>6</v>
       </c>
       <c r="L96" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M96" s="2" t="s">
-        <v>1057</v>
+        <v>1050</v>
       </c>
       <c r="N96" s="2" t="s">
         <v>411</v>
       </c>
       <c r="O96" s="2" t="s">
-        <v>1058</v>
+        <v>1051</v>
       </c>
       <c r="P96" s="2" t="s">
         <v>412</v>
@@ -9774,13 +9779,13 @@
         <v>414</v>
       </c>
       <c r="M97" s="2" t="s">
-        <v>1059</v>
+        <v>1052</v>
       </c>
       <c r="N97" s="2" t="s">
         <v>415</v>
       </c>
       <c r="O97" s="2" t="s">
-        <v>1060</v>
+        <v>1053</v>
       </c>
       <c r="P97" s="2" t="s">
         <v>416</v>
@@ -9821,16 +9826,16 @@
         <v>6</v>
       </c>
       <c r="L98" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M98" s="2" t="s">
-        <v>1061</v>
+        <v>1054</v>
       </c>
       <c r="N98" s="2" t="s">
         <v>418</v>
       </c>
       <c r="O98" s="2" t="s">
-        <v>1062</v>
+        <v>1055</v>
       </c>
       <c r="P98" s="2" t="s">
         <v>419</v>
@@ -9871,16 +9876,16 @@
         <v>6</v>
       </c>
       <c r="L99" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M99" s="2" t="s">
-        <v>1063</v>
+        <v>1056</v>
       </c>
       <c r="N99" s="2" t="s">
-        <v>1146</v>
+        <v>1139</v>
       </c>
       <c r="O99" s="2" t="s">
-        <v>1064</v>
+        <v>1057</v>
       </c>
       <c r="P99" s="2" t="s">
         <v>421</v>
@@ -9921,16 +9926,16 @@
         <v>6</v>
       </c>
       <c r="L100" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M100" s="2" t="s">
-        <v>1065</v>
+        <v>1058</v>
       </c>
       <c r="N100" s="2" t="s">
         <v>453</v>
       </c>
       <c r="O100" s="2" t="s">
-        <v>1066</v>
+        <v>1059</v>
       </c>
       <c r="P100" s="2" t="s">
         <v>454</v>
@@ -9971,16 +9976,16 @@
         <v>6</v>
       </c>
       <c r="L101" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M101" s="2" t="s">
-        <v>1067</v>
+        <v>1060</v>
       </c>
       <c r="N101" s="2" t="s">
         <v>423</v>
       </c>
       <c r="O101" s="2" t="s">
-        <v>1068</v>
+        <v>1061</v>
       </c>
       <c r="P101" s="2" t="s">
         <v>458</v>
@@ -10021,16 +10026,16 @@
         <v>6</v>
       </c>
       <c r="L102" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M102" s="2" t="s">
-        <v>1069</v>
+        <v>1062</v>
       </c>
       <c r="N102" s="2" t="s">
         <v>461</v>
       </c>
       <c r="O102" s="2" t="s">
-        <v>1070</v>
+        <v>1063</v>
       </c>
       <c r="P102" s="2" t="s">
         <v>462</v>
@@ -10071,16 +10076,16 @@
         <v>6</v>
       </c>
       <c r="L103" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M103" s="2" t="s">
-        <v>1071</v>
+        <v>1064</v>
       </c>
       <c r="N103" s="2" t="s">
         <v>466</v>
       </c>
       <c r="O103" s="2" t="s">
-        <v>1072</v>
+        <v>1065</v>
       </c>
       <c r="P103" s="2" t="s">
         <v>467</v>
@@ -10121,16 +10126,16 @@
         <v>471</v>
       </c>
       <c r="L104" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M104" s="2" t="s">
-        <v>1073</v>
+        <v>1066</v>
       </c>
       <c r="N104" s="2" t="s">
         <v>472</v>
       </c>
       <c r="O104" s="2" t="s">
-        <v>1074</v>
+        <v>1067</v>
       </c>
       <c r="P104" s="2" t="s">
         <v>473</v>
@@ -10171,16 +10176,16 @@
         <v>6</v>
       </c>
       <c r="L105" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M105" s="2" t="s">
-        <v>1075</v>
+        <v>1068</v>
       </c>
       <c r="N105" s="2" t="s">
-        <v>1156</v>
+        <v>1149</v>
       </c>
       <c r="O105" s="2" t="s">
-        <v>1076</v>
+        <v>1069</v>
       </c>
       <c r="P105" s="2" t="s">
         <v>477</v>
@@ -10221,16 +10226,16 @@
         <v>6</v>
       </c>
       <c r="L106" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M106" s="2" t="s">
-        <v>1077</v>
+        <v>1070</v>
       </c>
       <c r="N106" s="2" t="s">
-        <v>1139</v>
+        <v>1132</v>
       </c>
       <c r="O106" s="2" t="s">
-        <v>1078</v>
+        <v>1071</v>
       </c>
       <c r="P106" s="2" t="s">
         <v>480</v>
@@ -10271,16 +10276,16 @@
         <v>6</v>
       </c>
       <c r="L107" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M107" s="2" t="s">
-        <v>1079</v>
+        <v>1072</v>
       </c>
       <c r="N107" s="2" t="s">
         <v>483</v>
       </c>
       <c r="O107" s="2" t="s">
-        <v>1080</v>
+        <v>1073</v>
       </c>
       <c r="P107" s="2" t="s">
         <v>484</v>
@@ -10321,16 +10326,16 @@
         <v>6</v>
       </c>
       <c r="L108" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M108" s="2" t="s">
-        <v>1081</v>
+        <v>1074</v>
       </c>
       <c r="N108" s="2" t="s">
         <v>487</v>
       </c>
       <c r="O108" s="2" t="s">
-        <v>1082</v>
+        <v>1075</v>
       </c>
       <c r="P108" s="2" t="s">
         <v>488</v>
@@ -10371,16 +10376,16 @@
         <v>6</v>
       </c>
       <c r="L109" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M109" s="2" t="s">
-        <v>1083</v>
+        <v>1076</v>
       </c>
       <c r="N109" s="2" t="s">
         <v>491</v>
       </c>
       <c r="O109" s="2" t="s">
-        <v>1084</v>
+        <v>1077</v>
       </c>
       <c r="P109" s="2" t="s">
         <v>492</v>
@@ -10421,16 +10426,16 @@
         <v>6</v>
       </c>
       <c r="L110" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M110" s="2" t="s">
-        <v>1085</v>
+        <v>1078</v>
       </c>
       <c r="N110" s="2" t="s">
         <v>495</v>
       </c>
       <c r="O110" s="2" t="s">
-        <v>1086</v>
+        <v>1079</v>
       </c>
       <c r="P110" s="2" t="s">
         <v>496</v>
@@ -10471,16 +10476,16 @@
         <v>6</v>
       </c>
       <c r="L111" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M111" s="2" t="s">
-        <v>1087</v>
+        <v>1080</v>
       </c>
       <c r="N111" s="2" t="s">
         <v>499</v>
       </c>
       <c r="O111" s="2" t="s">
-        <v>1088</v>
+        <v>1081</v>
       </c>
       <c r="P111" s="2" t="s">
         <v>500</v>
@@ -10521,16 +10526,16 @@
         <v>503</v>
       </c>
       <c r="L112" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M112" s="2" t="s">
-        <v>1089</v>
+        <v>1082</v>
       </c>
       <c r="N112" s="2" t="s">
-        <v>1139</v>
+        <v>1132</v>
       </c>
       <c r="O112" s="2" t="s">
-        <v>1090</v>
+        <v>1083</v>
       </c>
       <c r="P112" s="2" t="s">
         <v>504</v>
@@ -10571,16 +10576,16 @@
         <v>508</v>
       </c>
       <c r="L113" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M113" s="2" t="s">
-        <v>1091</v>
+        <v>1084</v>
       </c>
       <c r="N113" s="2" t="s">
         <v>509</v>
       </c>
       <c r="O113" s="2" t="s">
-        <v>1092</v>
+        <v>1085</v>
       </c>
       <c r="P113" s="2" t="s">
         <v>510</v>
@@ -10621,16 +10626,16 @@
         <v>6</v>
       </c>
       <c r="L114" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M114" s="2" t="s">
-        <v>1093</v>
+        <v>1086</v>
       </c>
       <c r="N114" s="2" t="s">
         <v>514</v>
       </c>
       <c r="O114" s="2" t="s">
-        <v>1094</v>
+        <v>1087</v>
       </c>
       <c r="P114" s="2" t="s">
         <v>515</v>
@@ -10671,16 +10676,16 @@
         <v>6</v>
       </c>
       <c r="L115" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M115" s="2" t="s">
-        <v>1095</v>
+        <v>1088</v>
       </c>
       <c r="N115" s="2" t="s">
-        <v>1139</v>
+        <v>1132</v>
       </c>
       <c r="O115" s="2" t="s">
-        <v>1096</v>
+        <v>1089</v>
       </c>
       <c r="P115" s="2" t="s">
         <v>519</v>
@@ -10721,16 +10726,16 @@
         <v>6</v>
       </c>
       <c r="L116" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M116" s="2" t="s">
-        <v>1097</v>
+        <v>1090</v>
       </c>
       <c r="N116" s="2" t="s">
         <v>523</v>
       </c>
       <c r="O116" s="2" t="s">
-        <v>1098</v>
+        <v>1091</v>
       </c>
       <c r="P116" s="2" t="s">
         <v>524</v>
@@ -10771,16 +10776,16 @@
         <v>6</v>
       </c>
       <c r="L117" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M117" s="2" t="s">
-        <v>1099</v>
+        <v>1092</v>
       </c>
       <c r="N117" s="2" t="s">
         <v>527</v>
       </c>
       <c r="O117" s="2" t="s">
-        <v>1100</v>
+        <v>1093</v>
       </c>
       <c r="P117" s="2" t="s">
         <v>528</v>
@@ -10815,22 +10820,22 @@
         <v>5</v>
       </c>
       <c r="J118" s="2" t="s">
-        <v>1101</v>
+        <v>1094</v>
       </c>
       <c r="K118" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L118" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M118" s="2" t="s">
-        <v>1102</v>
+        <v>1095</v>
       </c>
       <c r="N118" s="2" t="s">
         <v>531</v>
       </c>
       <c r="O118" s="2" t="s">
-        <v>1103</v>
+        <v>1096</v>
       </c>
       <c r="P118" s="2" t="s">
         <v>532</v>
@@ -10871,16 +10876,16 @@
         <v>536</v>
       </c>
       <c r="L119" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M119" s="2" t="s">
-        <v>1157</v>
+        <v>1150</v>
       </c>
       <c r="N119" s="2" t="s">
         <v>537</v>
       </c>
       <c r="O119" s="2" t="s">
-        <v>1104</v>
+        <v>1097</v>
       </c>
       <c r="P119" s="2" t="s">
         <v>538</v>
@@ -10921,16 +10926,16 @@
         <v>542</v>
       </c>
       <c r="L120" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M120" s="2" t="s">
-        <v>1105</v>
+        <v>1098</v>
       </c>
       <c r="N120" s="2" t="s">
         <v>543</v>
       </c>
       <c r="O120" s="2" t="s">
-        <v>1106</v>
+        <v>1099</v>
       </c>
       <c r="P120" s="2" t="s">
         <v>544</v>
@@ -10971,16 +10976,16 @@
         <v>548</v>
       </c>
       <c r="L121" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M121" s="2" t="s">
-        <v>1107</v>
+        <v>1100</v>
       </c>
       <c r="N121" s="2" t="s">
         <v>549</v>
       </c>
       <c r="O121" s="2" t="s">
-        <v>1108</v>
+        <v>1101</v>
       </c>
       <c r="P121" s="2" t="s">
         <v>550</v>
@@ -11021,16 +11026,16 @@
         <v>6</v>
       </c>
       <c r="L122" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M122" s="2" t="s">
-        <v>1109</v>
+        <v>1102</v>
       </c>
       <c r="N122" s="2" t="s">
-        <v>1158</v>
+        <v>1151</v>
       </c>
       <c r="O122" s="2" t="s">
-        <v>1110</v>
+        <v>1103</v>
       </c>
       <c r="P122" s="2" t="s">
         <v>552</v>
@@ -11071,16 +11076,16 @@
         <v>6</v>
       </c>
       <c r="L123" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M123" s="2" t="s">
-        <v>1111</v>
+        <v>1104</v>
       </c>
       <c r="N123" s="2" t="s">
         <v>555</v>
       </c>
       <c r="O123" s="2" t="s">
-        <v>1112</v>
+        <v>1105</v>
       </c>
       <c r="P123" s="2" t="s">
         <v>556</v>
@@ -11121,16 +11126,16 @@
         <v>560</v>
       </c>
       <c r="L124" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M124" s="2" t="s">
-        <v>1113</v>
+        <v>1106</v>
       </c>
       <c r="N124" s="2" t="s">
         <v>561</v>
       </c>
       <c r="O124" s="2" t="s">
-        <v>1114</v>
+        <v>1107</v>
       </c>
       <c r="P124" s="2" t="s">
         <v>562</v>
@@ -11171,16 +11176,16 @@
         <v>6</v>
       </c>
       <c r="L125" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M125" s="2" t="s">
-        <v>1115</v>
+        <v>1108</v>
       </c>
       <c r="N125" s="2" t="s">
-        <v>1159</v>
+        <v>1152</v>
       </c>
       <c r="O125" s="2" t="s">
-        <v>1116</v>
+        <v>1109</v>
       </c>
       <c r="P125" s="2" t="s">
         <v>565</v>
@@ -11221,16 +11226,16 @@
         <v>6</v>
       </c>
       <c r="L126" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M126" s="2" t="s">
-        <v>1117</v>
+        <v>1110</v>
       </c>
       <c r="N126" s="2" t="s">
         <v>568</v>
       </c>
       <c r="O126" s="2" t="s">
-        <v>1118</v>
+        <v>1111</v>
       </c>
       <c r="P126" s="2" t="s">
         <v>569</v>
@@ -11271,16 +11276,16 @@
         <v>6</v>
       </c>
       <c r="L127" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M127" s="2" t="s">
-        <v>1119</v>
+        <v>1112</v>
       </c>
       <c r="N127" s="2" t="s">
         <v>572</v>
       </c>
       <c r="O127" s="2" t="s">
-        <v>1120</v>
+        <v>1113</v>
       </c>
       <c r="P127" s="2" t="s">
         <v>573</v>
@@ -11321,16 +11326,16 @@
         <v>578</v>
       </c>
       <c r="L128" s="2" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="M128" s="2" t="s">
-        <v>1121</v>
+        <v>1114</v>
       </c>
       <c r="N128" s="2" t="s">
-        <v>1139</v>
+        <v>1132</v>
       </c>
       <c r="O128" s="2" t="s">
-        <v>1122</v>
+        <v>1115</v>
       </c>
       <c r="P128" s="2" t="s">
         <v>579</v>

</xml_diff>